<commit_message>
Update TC_ID Excel SCD0017 until SCD0025 and Update TC_ID Solution SCD0006 until SCD0025
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0017-001 - Pengajuan customer flagging.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0017-001 - Pengajuan customer flagging.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79388DFA-93C4-4C0A-93CA-BCEA285137BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C433C4-727D-4B54-9D0B-7F3D9D3940F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SCD0271" sheetId="2" r:id="rId1"/>
+    <sheet name="SCD0017" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -95,9 +95,6 @@
     <t>FLAGGING</t>
   </si>
   <si>
-    <t>DGS-286</t>
-  </si>
-  <si>
     <t>Pengajuan customer flagging</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>Update Status Flagging menjadi Menunggu Approval SPV/Penyelia</t>
+  </si>
+  <si>
+    <t>SCD0017-001</t>
   </si>
 </sst>
 </file>
@@ -590,14 +590,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.5703125" bestFit="1" customWidth="1"/>
@@ -670,31 +670,31 @@
         <v>17</v>
       </c>
       <c r="Q1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" t="s">
         <v>30</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>31</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>32</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>33</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>34</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>35</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="102" x14ac:dyDescent="0.25">
@@ -702,16 +702,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>23</v>
       </c>
       <c r="F2" s="12">
         <v>23320</v>
@@ -730,7 +730,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M2" s="12">
         <v>10187811885</v>
@@ -750,16 +750,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>22</v>
-      </c>
       <c r="D3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="11"/>
@@ -772,20 +772,20 @@
       <c r="N3" s="13"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S3" s="10"/>
       <c r="T3" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="V3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="V3" s="10" t="s">
-        <v>39</v>
-      </c>
       <c r="W3" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="102" x14ac:dyDescent="0.25">
@@ -793,16 +793,16 @@
         <v>0</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>23</v>
       </c>
       <c r="F4" s="12">
         <v>23320</v>
@@ -821,7 +821,7 @@
         <v>20</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M4" s="12">
         <v>10187811885</v>

</xml_diff>